<commit_message>
fixed view add new icon and a lot of refactoring
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Apprentices.xlsx
+++ b/src/main/resources/excel/Apprentices.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,24 @@
   </si>
   <si>
     <t>2017-05-05</t>
+  </si>
+  <si>
+    <t>NBV6qZjWZyYdi1kAKln+46n07FtdDKgPUaweBSoWUdDlqqPbKDPFiVtShe0dg60wXNfW5+w0O9sUi/gflkooQh+998aT7iMKOMuYQhTlX89A2mGRO/mH3pXljHU4BubEPP4YZqrW+9qCA8m+RtzjXpOCDeaIe99kOQQibe0H5gw=</t>
+  </si>
+  <si>
+    <t>bfXCkN6OI/k6lKWAlmqlxuZKUYjC2v+ppzktjsx7WJsblgWbdwmWOq8at1DIGO3kZBqLqbhgzuQQyGdNJMaiVr3r3ZrlumL+y0snAonQpS9CvdUhgbCghHQy8ktzp4pw11GsQoGTxQFI/hOvr/SsGhZiBSWteuJt/KceDVJKN/I=</t>
+  </si>
+  <si>
+    <t>d+eFclghqlZ51NbGIVZg2UhdyCNJj0Mo+MvGLF6ry1vUEgcPtJuuLfdsGdQ8L2XJWjlxBqWlsDwm7p8JOBoHbm+OHQfBMA582n3NF2irdMFwwsKQ6ja9D7dFBexBOJgWnJWlZlaP/cOzhdJbvVY/GGxu8q/jbqmk7ZGG3IbpO3s=</t>
+  </si>
+  <si>
+    <t>CLS</t>
+  </si>
+  <si>
+    <t>WS5sTbLXc36YJqMXyGb+souFJzoMuKvRnkr0gZ9b+mEw0hg0QVVpEPp7/usNy3OWD29YcZri7SpvuezsDXwAm/sQ4lTdXywp777wNGNBwSZtLYlvT+Q6IxnP+vbVllijWQyedMmjS6hYGG47fHFzJEfEcHO2UF+Zge31345kM+Y=</t>
+  </si>
+  <si>
+    <t>2017-05-23</t>
   </si>
 </sst>
 </file>
@@ -98,15 +116,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.16796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.0625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.54296875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.98828125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.359375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="196.37109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="189.62109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="190.92578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.42578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="194.62890625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -143,6 +164,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>